<commit_message>
more work on final project
</commit_message>
<xml_diff>
--- a/BINF620-R Projects/Final Project/NSCH_2022_Variable labels.xlsx
+++ b/BINF620-R Projects/Final Project/NSCH_2022_Variable labels.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://udwinprod-my.sharepoint.com/personal/assmith_udel_edu/Documents/R Projects/BINF620/BINF620-R Projects/Final Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="38" documentId="13_ncr:1_{9001EE24-37D9-42AB-9079-2AB75D2F548C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{47324A96-F8B6-4B00-A507-90404006076F}"/>
+  <xr:revisionPtr revIDLastSave="43" documentId="13_ncr:1_{9001EE24-37D9-42AB-9079-2AB75D2F548C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{98B3324C-04C4-4C3C-9F3C-DA5C8BF7B132}"/>
   <bookViews>
-    <workbookView xWindow="2412" yWindow="-17388" windowWidth="30936" windowHeight="16776" activeTab="1" xr2:uid="{24CD0A18-0D74-4436-8BB0-CF90BAB9E784}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" activeTab="4" xr2:uid="{24CD0A18-0D74-4436-8BB0-CF90BAB9E784}"/>
   </bookViews>
   <sheets>
     <sheet name="Raw Variables" sheetId="1" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2769" uniqueCount="1971">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2771" uniqueCount="1972">
   <si>
     <t>FIPSST</t>
   </si>
@@ -6052,6 +6052,9 @@
 3 "1-2 times per month" 
 4 "1-2 times per week" 
 5 "Almost every day"</t>
+  </si>
+  <si>
+    <t>MHealthConcern ~ HHCOUNT + K8Q35 + TalkAbout_22 + RACE + NbhdSupp_22 + NbhdSafe_22 + ACE2more6HH_22 + INQ_INCOME</t>
   </si>
 </sst>
 </file>
@@ -6168,6 +6171,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
@@ -14051,9 +14058,9 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:H231"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A185" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C247" sqref="C247"/>
+      <selection pane="bottomLeft" activeCell="B242" sqref="B242"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -17305,10 +17312,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7B17E8F-9228-4F03-B401-83ABEE385989}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -17379,6 +17386,14 @@
       <c r="E4" s="5"/>
       <c r="F4" s="4" t="s">
         <v>1969</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+      <c r="C5" t="s">
+        <v>1881</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>1971</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Final Assignment 8 then supporting code for final project
</commit_message>
<xml_diff>
--- a/BINF620-R Projects/Final Project/NSCH_2022_Variable labels.xlsx
+++ b/BINF620-R Projects/Final Project/NSCH_2022_Variable labels.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://udwinprod-my.sharepoint.com/personal/assmith_udel_edu/Documents/R Projects/BINF620/BINF620-R Projects/Final Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="43" documentId="13_ncr:1_{9001EE24-37D9-42AB-9079-2AB75D2F548C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{98B3324C-04C4-4C3C-9F3C-DA5C8BF7B132}"/>
+  <xr:revisionPtr revIDLastSave="299" documentId="13_ncr:1_{9001EE24-37D9-42AB-9079-2AB75D2F548C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A6744339-B37D-46D1-AA95-078E73CCBB50}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" activeTab="4" xr2:uid="{24CD0A18-0D74-4436-8BB0-CF90BAB9E784}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" activeTab="1" xr2:uid="{24CD0A18-0D74-4436-8BB0-CF90BAB9E784}"/>
   </bookViews>
   <sheets>
     <sheet name="Raw Variables" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <sheet name="Idea Board" sheetId="7" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Dictionary!$A$1:$H$231</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Dictionary!$A$1:$I$231</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Raw Variables'!$A$1:$B$934</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Statistical Methods'!$A$1:$B$1</definedName>
   </definedNames>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2771" uniqueCount="1972">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2999" uniqueCount="1984">
   <si>
     <t>FIPSST</t>
   </si>
@@ -6055,6 +6055,55 @@
   </si>
   <si>
     <t>MHealthConcern ~ HHCOUNT + K8Q35 + TalkAbout_22 + RACE + NbhdSupp_22 + NbhdSafe_22 + ACE2more6HH_22 + INQ_INCOME</t>
+  </si>
+  <si>
+    <t>1 = Less than 1 hour
+2 = 1 hour
+3 = 2 hours
+4 = 3 hours
+5 = 4 or more hours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 Excellent or very good 2 Good 3 Fair or poor </t>
+  </si>
+  <si>
+    <t>For Calculation</t>
+  </si>
+  <si>
+    <t>Models Used In</t>
+  </si>
+  <si>
+    <t>Neighborhood / Activities / Support Model | Model1</t>
+  </si>
+  <si>
+    <t>Family / History Model | Model2</t>
+  </si>
+  <si>
+    <t># Adverse Events / Friends Model | Model3</t>
+  </si>
+  <si>
+    <t># Combined Model | Model4</t>
+  </si>
+  <si>
+    <t>"OutcomeVariable ~ HHCOUNT+PHYSACTIV+K8Q35+mentor_22+ShareIdeas_22+
+          ScreenTime_22+ACE4ctCom_22+ AftSchAct_22+NbhdSupp_22+NbhdSafe_22"</t>
+  </si>
+  <si>
+    <t>"OutcomeVariable ~ BORNUSA+ACE12+ACE11+K10Q40_R+
+          age3_22+sex_22+MotherMH_22+FatherMH_22+SC_RACE_R+
+          EventPart_22+mentor_22+ACE2more11_22+ACE6ctHH_22"</t>
+  </si>
+  <si>
+    <t>"OutcomeVariable ~ HHCOUNT+BORNUSA+K8Q35+ACE12+ACE11+
+          age3_22+SC_RACE_R+bully_22+bullied_22+AftSchAct_22+
+          EventPart_22+mentor_22+ShareIdeas_22"</t>
+  </si>
+  <si>
+    <t>"OutcomeVariable ~ HHCOUNT+BORNUSA+K8Q35+ACE12+ACE11+K10Q40_R+PHYSACTIV+
+          age3_22+sex_22+MotherMH_22+FatherMH_22+ScreenTime_22+
+          ACEct11_22+ACE4ctCom_22+SC_RACE_R+bully_22+bullied_22+AftSchAct_22+
+          EventPart_22+mentor_22+ShareIdeas_22+ACE2more11_22+ACE6ctHH_22+
+          NbhdSupp_22+NbhdSafe_22"</t>
   </si>
 </sst>
 </file>
@@ -6125,7 +6174,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -6139,13 +6188,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -14056,27 +14106,28 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDF76284-18C6-40F6-BB15-A93600E21133}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:H231"/>
+  <dimension ref="A1:I231"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A185" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B242" sqref="B242"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C237" sqref="C237"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="23.265625" customWidth="1"/>
-    <col min="2" max="2" width="96.6640625" customWidth="1"/>
-    <col min="3" max="3" width="50.3984375" customWidth="1"/>
-    <col min="4" max="4" width="25" customWidth="1"/>
-    <col min="5" max="5" width="19" customWidth="1"/>
+    <col min="1" max="1" width="23.265625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="41" customWidth="1"/>
+    <col min="3" max="3" width="35.19921875" customWidth="1"/>
+    <col min="4" max="4" width="16.53125" customWidth="1"/>
+    <col min="5" max="5" width="16.3984375" customWidth="1"/>
     <col min="6" max="6" width="14.265625" customWidth="1"/>
     <col min="7" max="7" width="12.1328125" customWidth="1"/>
-    <col min="8" max="8" width="73.73046875" customWidth="1"/>
+    <col min="8" max="8" width="18.59765625" customWidth="1"/>
+    <col min="9" max="9" width="73.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="10" t="s">
         <v>1860</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -14098,11 +14149,14 @@
         <v>1872</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>1975</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>1914</v>
       </c>
     </row>
-    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A2" s="9" t="s">
         <v>14</v>
       </c>
       <c r="B2" t="s">
@@ -14115,11 +14169,11 @@
         <v>1939</v>
       </c>
       <c r="F2" t="s">
-        <v>1869</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="7" t="s">
+        <v>1871</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="9" t="s">
         <v>94</v>
       </c>
       <c r="B3" t="s">
@@ -14131,9 +14185,12 @@
       <c r="E3" t="s">
         <v>1943</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="7" t="s">
+      <c r="F3" t="s">
+        <v>1869</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="9" t="s">
         <v>104</v>
       </c>
       <c r="B4" t="s">
@@ -14145,8 +14202,14 @@
       <c r="E4" t="s">
         <v>1937</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F4" t="s">
+        <v>1870</v>
+      </c>
+      <c r="G4" t="s">
+        <v>1874</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>106</v>
       </c>
@@ -14159,9 +14222,12 @@
       <c r="E5" t="s">
         <v>1937</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="7" t="s">
+      <c r="F5" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A6" s="9" t="s">
         <v>166</v>
       </c>
       <c r="B6" t="s">
@@ -14171,14 +14237,11 @@
         <v>171</v>
       </c>
       <c r="F6" t="s">
-        <v>1870</v>
-      </c>
-      <c r="G6" t="s">
-        <v>1873</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A7" s="9" t="s">
         <v>168</v>
       </c>
       <c r="B7" t="s">
@@ -14187,9 +14250,12 @@
       <c r="E7" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="7" t="s">
+      <c r="F7" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A8" s="9" t="s">
         <v>170</v>
       </c>
       <c r="B8" t="s">
@@ -14199,14 +14265,11 @@
         <v>171</v>
       </c>
       <c r="F8" t="s">
-        <v>1870</v>
-      </c>
-      <c r="G8" t="s">
-        <v>1873</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A9" s="9" t="s">
         <v>172</v>
       </c>
       <c r="B9" t="s">
@@ -14215,8 +14278,11 @@
       <c r="E9" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F9" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>184</v>
       </c>
@@ -14226,8 +14292,11 @@
       <c r="E10" t="s">
         <v>1935</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F10" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>198</v>
       </c>
@@ -14237,8 +14306,11 @@
       <c r="E11" t="s">
         <v>1939</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F11" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>214</v>
       </c>
@@ -14257,11 +14329,11 @@
       <c r="F12" t="s">
         <v>1868</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
         <v>1915</v>
       </c>
     </row>
-    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>216</v>
       </c>
@@ -14281,7 +14353,7 @@
         <v>1868</v>
       </c>
     </row>
-    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>218</v>
       </c>
@@ -14301,7 +14373,7 @@
         <v>1868</v>
       </c>
     </row>
-    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>242</v>
       </c>
@@ -14311,8 +14383,11 @@
       <c r="E15" t="s">
         <v>1944</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F15" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>244</v>
       </c>
@@ -14322,8 +14397,11 @@
       <c r="E16" t="s">
         <v>1944</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F16" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>246</v>
       </c>
@@ -14333,8 +14411,11 @@
       <c r="E17" t="s">
         <v>1944</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F17" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>248</v>
       </c>
@@ -14344,8 +14425,11 @@
       <c r="E18" t="s">
         <v>1944</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F18" t="s">
+        <v>1869</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>250</v>
       </c>
@@ -14355,8 +14439,11 @@
       <c r="E19" t="s">
         <v>1944</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F19" t="s">
+        <v>1869</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>252</v>
       </c>
@@ -14366,8 +14453,11 @@
       <c r="E20" t="s">
         <v>1944</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F20" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>254</v>
       </c>
@@ -14377,8 +14467,11 @@
       <c r="E21" t="s">
         <v>1944</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F21" t="s">
+        <v>1869</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>256</v>
       </c>
@@ -14388,9 +14481,12 @@
       <c r="E22" t="s">
         <v>1944</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A23" t="s">
+      <c r="F22" t="s">
+        <v>1869</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A23" s="9" t="s">
         <v>388</v>
       </c>
       <c r="B23" t="s">
@@ -14399,9 +14495,15 @@
       <c r="E23" t="s">
         <v>1943</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A24" t="s">
+      <c r="F23" t="s">
+        <v>1870</v>
+      </c>
+      <c r="G23" t="s">
+        <v>1874</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A24" s="9" t="s">
         <v>390</v>
       </c>
       <c r="B24" t="s">
@@ -14411,10 +14513,13 @@
         <v>1945</v>
       </c>
       <c r="F24" t="s">
-        <v>1869</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+        <v>1870</v>
+      </c>
+      <c r="G24" t="s">
+        <v>1874</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>392</v>
       </c>
@@ -14424,8 +14529,11 @@
       <c r="E25" t="s">
         <v>1945</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F25" t="s">
+        <v>1869</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>394</v>
       </c>
@@ -14435,8 +14543,11 @@
       <c r="E26" t="s">
         <v>1945</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F26" t="s">
+        <v>1869</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>396</v>
       </c>
@@ -14446,8 +14557,11 @@
       <c r="E27" t="s">
         <v>1945</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F27" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>398</v>
       </c>
@@ -14461,7 +14575,7 @@
         <v>1869</v>
       </c>
     </row>
-    <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>400</v>
       </c>
@@ -14471,8 +14585,11 @@
       <c r="E29" t="s">
         <v>1945</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F29" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>402</v>
       </c>
@@ -14482,8 +14599,11 @@
       <c r="E30" t="s">
         <v>1945</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F30" t="s">
+        <v>1869</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>404</v>
       </c>
@@ -14493,8 +14613,11 @@
       <c r="E31" t="s">
         <v>1945</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F31" t="s">
+        <v>1869</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>406</v>
       </c>
@@ -14503,6 +14626,9 @@
       </c>
       <c r="E32" t="s">
         <v>1945</v>
+      </c>
+      <c r="F32" t="s">
+        <v>1868</v>
       </c>
     </row>
     <row r="33" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
@@ -14515,6 +14641,9 @@
       <c r="E33" t="s">
         <v>1946</v>
       </c>
+      <c r="F33" t="s">
+        <v>1868</v>
+      </c>
     </row>
     <row r="34" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
@@ -14540,6 +14669,9 @@
       <c r="E35" t="s">
         <v>1946</v>
       </c>
+      <c r="F35" t="s">
+        <v>1868</v>
+      </c>
     </row>
     <row r="36" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
@@ -14551,6 +14683,9 @@
       <c r="E36" t="s">
         <v>1946</v>
       </c>
+      <c r="F36" t="s">
+        <v>1868</v>
+      </c>
     </row>
     <row r="37" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
@@ -14562,6 +14697,9 @@
       <c r="E37" t="s">
         <v>1946</v>
       </c>
+      <c r="F37" t="s">
+        <v>1868</v>
+      </c>
     </row>
     <row r="38" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
@@ -14573,6 +14711,9 @@
       <c r="E38" t="s">
         <v>1946</v>
       </c>
+      <c r="F38" t="s">
+        <v>1868</v>
+      </c>
     </row>
     <row r="39" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
@@ -14585,7 +14726,7 @@
         <v>1946</v>
       </c>
       <c r="F39" t="s">
-        <v>1869</v>
+        <v>1868</v>
       </c>
     </row>
     <row r="40" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
@@ -14599,11 +14740,11 @@
         <v>1946</v>
       </c>
       <c r="F40" t="s">
-        <v>1869</v>
+        <v>1868</v>
       </c>
     </row>
     <row r="41" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A41" t="s">
+      <c r="A41" s="9" t="s">
         <v>464</v>
       </c>
       <c r="B41" t="s">
@@ -14612,9 +14753,15 @@
       <c r="E41" t="s">
         <v>1946</v>
       </c>
+      <c r="F41" t="s">
+        <v>1870</v>
+      </c>
+      <c r="G41" t="s">
+        <v>1874</v>
+      </c>
     </row>
     <row r="42" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A42" t="s">
+      <c r="A42" s="9" t="s">
         <v>466</v>
       </c>
       <c r="B42" t="s">
@@ -14623,9 +14770,15 @@
       <c r="E42" t="s">
         <v>1946</v>
       </c>
+      <c r="F42" t="s">
+        <v>1870</v>
+      </c>
+      <c r="G42" t="s">
+        <v>1874</v>
+      </c>
     </row>
     <row r="43" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A43" s="7" t="s">
+      <c r="A43" s="9" t="s">
         <v>660</v>
       </c>
       <c r="B43" t="s">
@@ -14633,6 +14786,9 @@
       </c>
       <c r="E43" t="s">
         <v>1937</v>
+      </c>
+      <c r="F43" t="s">
+        <v>1869</v>
       </c>
     </row>
     <row r="44" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
@@ -14645,6 +14801,9 @@
       <c r="E44" t="s">
         <v>1933</v>
       </c>
+      <c r="F44" t="s">
+        <v>1868</v>
+      </c>
     </row>
     <row r="45" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
@@ -14656,9 +14815,12 @@
       <c r="E45" t="s">
         <v>1933</v>
       </c>
+      <c r="F45" t="s">
+        <v>1868</v>
+      </c>
     </row>
     <row r="46" spans="1:7" ht="57" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A46" s="7" t="s">
+      <c r="A46" s="9" t="s">
         <v>682</v>
       </c>
       <c r="B46" t="s">
@@ -14690,6 +14852,9 @@
       <c r="E47" t="s">
         <v>1939</v>
       </c>
+      <c r="F47" t="s">
+        <v>1868</v>
+      </c>
     </row>
     <row r="48" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
@@ -14701,8 +14866,11 @@
       <c r="E48" t="s">
         <v>1939</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F48" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
         <v>687</v>
       </c>
@@ -14715,11 +14883,8 @@
       <c r="F49" t="s">
         <v>1869</v>
       </c>
-      <c r="G49" t="s">
-        <v>1874</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="50" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
         <v>689</v>
       </c>
@@ -14729,22 +14894,28 @@
       <c r="E50" t="s">
         <v>1934</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A51" t="s">
+      <c r="F50" t="s">
+        <v>1869</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="71.25" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A51" s="9" t="s">
         <v>691</v>
       </c>
       <c r="B51" t="s">
         <v>692</v>
       </c>
+      <c r="C51" s="4" t="s">
+        <v>1972</v>
+      </c>
       <c r="E51" t="s">
         <v>1934</v>
       </c>
       <c r="F51" t="s">
-        <v>1869</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
         <v>789</v>
       </c>
@@ -14757,11 +14928,8 @@
       <c r="F52" t="s">
         <v>1869</v>
       </c>
-      <c r="G52" t="s">
-        <v>1874</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="53" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
         <v>817</v>
       </c>
@@ -14771,8 +14939,11 @@
       <c r="E53" t="s">
         <v>1939</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F53" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
         <v>949</v>
       </c>
@@ -14782,8 +14953,11 @@
       <c r="E54" t="s">
         <v>1947</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F54" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
         <v>951</v>
       </c>
@@ -14793,8 +14967,11 @@
       <c r="E55" t="s">
         <v>1947</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F55" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
         <v>953</v>
       </c>
@@ -14804,8 +14981,11 @@
       <c r="E56" t="s">
         <v>1947</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F56" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
         <v>955</v>
       </c>
@@ -14815,8 +14995,11 @@
       <c r="E57" t="s">
         <v>1947</v>
       </c>
-    </row>
-    <row r="58" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F57" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
         <v>957</v>
       </c>
@@ -14826,8 +15009,11 @@
       <c r="E58" t="s">
         <v>1947</v>
       </c>
-    </row>
-    <row r="59" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F58" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
         <v>959</v>
       </c>
@@ -14837,8 +15023,11 @@
       <c r="E59" t="s">
         <v>1947</v>
       </c>
-    </row>
-    <row r="60" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F59" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
         <v>961</v>
       </c>
@@ -14848,8 +15037,11 @@
       <c r="E60" t="s">
         <v>1939</v>
       </c>
-    </row>
-    <row r="61" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F60" t="s">
+        <v>1869</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
         <v>963</v>
       </c>
@@ -14859,8 +15051,11 @@
       <c r="E61" t="s">
         <v>1939</v>
       </c>
-    </row>
-    <row r="62" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F61" t="s">
+        <v>1869</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
         <v>965</v>
       </c>
@@ -14874,7 +15069,7 @@
         <v>1869</v>
       </c>
     </row>
-    <row r="63" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
         <v>967</v>
       </c>
@@ -14884,8 +15079,11 @@
       <c r="E63" t="s">
         <v>1940</v>
       </c>
-    </row>
-    <row r="64" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F63" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
         <v>969</v>
       </c>
@@ -14895,8 +15093,11 @@
       <c r="E64" t="s">
         <v>1940</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F64" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
         <v>971</v>
       </c>
@@ -14906,8 +15107,11 @@
       <c r="E65" t="s">
         <v>1940</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F65" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
         <v>973</v>
       </c>
@@ -14917,8 +15121,11 @@
       <c r="E66" t="s">
         <v>1940</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F66" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
         <v>975</v>
       </c>
@@ -14928,8 +15135,11 @@
       <c r="E67" t="s">
         <v>1940</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F67" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
         <v>977</v>
       </c>
@@ -14939,9 +15149,12 @@
       <c r="E68" t="s">
         <v>1938</v>
       </c>
-    </row>
-    <row r="69" spans="1:6" ht="42.75" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A69" t="s">
+      <c r="F68" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" ht="42.75" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A69" s="9" t="s">
         <v>979</v>
       </c>
       <c r="B69" t="s">
@@ -14957,10 +15170,13 @@
         <v>1939</v>
       </c>
       <c r="F69" t="s">
-        <v>1869</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+        <v>1870</v>
+      </c>
+      <c r="G69" t="s">
+        <v>1874</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
         <v>981</v>
       </c>
@@ -14974,8 +15190,8 @@
         <v>1869</v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A71" t="s">
+    <row r="71" spans="1:7" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A71" s="9" t="s">
         <v>983</v>
       </c>
       <c r="B71" t="s">
@@ -14991,10 +15207,13 @@
         <v>1939</v>
       </c>
       <c r="F71" t="s">
-        <v>1869</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+        <v>1870</v>
+      </c>
+      <c r="G71" t="s">
+        <v>1874</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
         <v>985</v>
       </c>
@@ -15007,8 +15226,11 @@
       <c r="E72" t="s">
         <v>1940</v>
       </c>
-    </row>
-    <row r="73" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F72" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
         <v>987</v>
       </c>
@@ -15021,8 +15243,11 @@
       <c r="E73" t="s">
         <v>1940</v>
       </c>
-    </row>
-    <row r="74" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F73" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
         <v>988</v>
       </c>
@@ -15032,8 +15257,11 @@
       <c r="E74" t="s">
         <v>1940</v>
       </c>
-    </row>
-    <row r="75" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F74" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
         <v>990</v>
       </c>
@@ -15043,8 +15271,11 @@
       <c r="E75" t="s">
         <v>1935</v>
       </c>
-    </row>
-    <row r="76" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F75" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
         <v>992</v>
       </c>
@@ -15054,8 +15285,11 @@
       <c r="E76" t="s">
         <v>1935</v>
       </c>
-    </row>
-    <row r="77" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F76" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
         <v>994</v>
       </c>
@@ -15065,8 +15299,11 @@
       <c r="E77" t="s">
         <v>1935</v>
       </c>
-    </row>
-    <row r="78" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F77" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
         <v>996</v>
       </c>
@@ -15076,8 +15313,11 @@
       <c r="E78" t="s">
         <v>1937</v>
       </c>
-    </row>
-    <row r="79" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F78" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
         <v>998</v>
       </c>
@@ -15087,8 +15327,11 @@
       <c r="E79" t="s">
         <v>1947</v>
       </c>
-    </row>
-    <row r="80" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F79" t="s">
+        <v>1869</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
         <v>1000</v>
       </c>
@@ -15097,6 +15340,9 @@
       </c>
       <c r="E80" t="s">
         <v>1947</v>
+      </c>
+      <c r="F80" t="s">
+        <v>1868</v>
       </c>
     </row>
     <row r="81" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
@@ -15109,6 +15355,9 @@
       <c r="E81" t="s">
         <v>1935</v>
       </c>
+      <c r="F81" t="s">
+        <v>1868</v>
+      </c>
     </row>
     <row r="82" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
@@ -15120,6 +15369,9 @@
       <c r="E82" t="s">
         <v>1939</v>
       </c>
+      <c r="F82" t="s">
+        <v>1868</v>
+      </c>
     </row>
     <row r="83" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
@@ -15134,9 +15386,6 @@
       <c r="F83" t="s">
         <v>1869</v>
       </c>
-      <c r="G83" t="s">
-        <v>1873</v>
-      </c>
     </row>
     <row r="84" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
@@ -15151,9 +15400,6 @@
       <c r="F84" t="s">
         <v>1869</v>
       </c>
-      <c r="G84" t="s">
-        <v>1873</v>
-      </c>
     </row>
     <row r="85" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
@@ -15184,25 +15430,43 @@
       </c>
     </row>
     <row r="87" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A87" t="s">
+      <c r="A87" s="9" t="s">
         <v>1629</v>
       </c>
       <c r="B87" t="s">
         <v>1630</v>
       </c>
+      <c r="C87" t="s">
+        <v>1973</v>
+      </c>
       <c r="E87" t="s">
         <v>1935</v>
       </c>
+      <c r="F87" t="s">
+        <v>1870</v>
+      </c>
+      <c r="G87" t="s">
+        <v>1874</v>
+      </c>
     </row>
     <row r="88" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A88" t="s">
+      <c r="A88" s="9" t="s">
         <v>1631</v>
       </c>
       <c r="B88" t="s">
         <v>1632</v>
       </c>
+      <c r="C88" t="s">
+        <v>1973</v>
+      </c>
       <c r="E88" t="s">
         <v>1935</v>
+      </c>
+      <c r="F88" t="s">
+        <v>1870</v>
+      </c>
+      <c r="G88" t="s">
+        <v>1874</v>
       </c>
     </row>
     <row r="89" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
@@ -15215,6 +15479,9 @@
       <c r="E89" t="s">
         <v>1935</v>
       </c>
+      <c r="F89" t="s">
+        <v>1869</v>
+      </c>
     </row>
     <row r="90" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A90" t="s">
@@ -15226,9 +15493,12 @@
       <c r="E90" t="s">
         <v>1935</v>
       </c>
+      <c r="F90" t="s">
+        <v>1869</v>
+      </c>
     </row>
     <row r="91" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A91" t="s">
+      <c r="A91" s="9" t="s">
         <v>1655</v>
       </c>
       <c r="B91" t="s">
@@ -15236,6 +15506,12 @@
       </c>
       <c r="E91" t="s">
         <v>1934</v>
+      </c>
+      <c r="F91" t="s">
+        <v>1870</v>
+      </c>
+      <c r="G91" t="s">
+        <v>1874</v>
       </c>
     </row>
     <row r="92" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
@@ -15248,6 +15524,9 @@
       <c r="E92" t="s">
         <v>1946</v>
       </c>
+      <c r="F92" t="s">
+        <v>1868</v>
+      </c>
     </row>
     <row r="93" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A93" t="s">
@@ -15259,6 +15538,9 @@
       <c r="E93" t="s">
         <v>1946</v>
       </c>
+      <c r="F93" t="s">
+        <v>1868</v>
+      </c>
     </row>
     <row r="94" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A94" t="s">
@@ -15270,6 +15552,9 @@
       <c r="E94" t="s">
         <v>1946</v>
       </c>
+      <c r="F94" t="s">
+        <v>1868</v>
+      </c>
     </row>
     <row r="95" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A95" t="s">
@@ -15281,6 +15566,9 @@
       <c r="E95" t="s">
         <v>1946</v>
       </c>
+      <c r="F95" t="s">
+        <v>1868</v>
+      </c>
     </row>
     <row r="96" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A96" t="s">
@@ -15292,8 +15580,11 @@
       <c r="E96" t="s">
         <v>1946</v>
       </c>
-    </row>
-    <row r="97" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F96" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A97" t="s">
         <v>1684</v>
       </c>
@@ -15303,8 +15594,11 @@
       <c r="E97" t="s">
         <v>1946</v>
       </c>
-    </row>
-    <row r="98" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F97" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A98" t="s">
         <v>1686</v>
       </c>
@@ -15314,8 +15608,11 @@
       <c r="E98" t="s">
         <v>1946</v>
       </c>
-    </row>
-    <row r="99" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F98" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A99" t="s">
         <v>1688</v>
       </c>
@@ -15325,8 +15622,11 @@
       <c r="E99" t="s">
         <v>1946</v>
       </c>
-    </row>
-    <row r="100" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F99" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A100" t="s">
         <v>1690</v>
       </c>
@@ -15336,8 +15636,11 @@
       <c r="E100" t="s">
         <v>1946</v>
       </c>
-    </row>
-    <row r="101" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F100" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A101" t="s">
         <v>1692</v>
       </c>
@@ -15347,9 +15650,12 @@
       <c r="E101" t="s">
         <v>1946</v>
       </c>
-    </row>
-    <row r="102" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A102" s="7" t="s">
+      <c r="F101" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A102" s="9" t="s">
         <v>1694</v>
       </c>
       <c r="B102" t="s">
@@ -15358,8 +15664,14 @@
       <c r="E102" t="s">
         <v>1946</v>
       </c>
-    </row>
-    <row r="103" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F102" t="s">
+        <v>1870</v>
+      </c>
+      <c r="G102" t="s">
+        <v>1874</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A103" t="s">
         <v>1776</v>
       </c>
@@ -15369,9 +15681,12 @@
       <c r="E103" t="s">
         <v>1943</v>
       </c>
-    </row>
-    <row r="104" spans="1:6" ht="42.75" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A104" s="7" t="s">
+      <c r="F103" t="s">
+        <v>1869</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A104" s="9" t="s">
         <v>494</v>
       </c>
       <c r="B104" t="s">
@@ -15383,9 +15698,12 @@
       <c r="E104" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="105" spans="1:6" ht="42.75" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A105" s="7" t="s">
+      <c r="F104" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A105" s="9" t="s">
         <v>496</v>
       </c>
       <c r="B105" t="s">
@@ -15398,10 +15716,10 @@
         <v>171</v>
       </c>
       <c r="F105" t="s">
-        <v>1869</v>
-      </c>
-    </row>
-    <row r="106" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A106" t="s">
         <v>588</v>
       </c>
@@ -15411,8 +15729,11 @@
       <c r="E106" t="s">
         <v>1941</v>
       </c>
-    </row>
-    <row r="107" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F106" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A107" t="s">
         <v>590</v>
       </c>
@@ -15422,8 +15743,11 @@
       <c r="E107" t="s">
         <v>1941</v>
       </c>
-    </row>
-    <row r="108" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F107" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A108" t="s">
         <v>592</v>
       </c>
@@ -15433,8 +15757,11 @@
       <c r="E108" t="s">
         <v>1941</v>
       </c>
-    </row>
-    <row r="109" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F108" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A109" t="s">
         <v>594</v>
       </c>
@@ -15444,8 +15771,11 @@
       <c r="E109" t="s">
         <v>1941</v>
       </c>
-    </row>
-    <row r="110" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F109" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A110" t="s">
         <v>596</v>
       </c>
@@ -15455,8 +15785,11 @@
       <c r="E110" t="s">
         <v>1941</v>
       </c>
-    </row>
-    <row r="111" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F110" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A111" t="s">
         <v>598</v>
       </c>
@@ -15466,8 +15799,11 @@
       <c r="E111" t="s">
         <v>1941</v>
       </c>
-    </row>
-    <row r="112" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F111" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A112" t="s">
         <v>600</v>
       </c>
@@ -15478,10 +15814,10 @@
         <v>1941</v>
       </c>
       <c r="F112" t="s">
-        <v>1869</v>
-      </c>
-    </row>
-    <row r="113" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
       <c r="A113" t="s">
         <v>602</v>
       </c>
@@ -15491,8 +15827,11 @@
       <c r="E113" t="s">
         <v>1941</v>
       </c>
-    </row>
-    <row r="114" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F113" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
       <c r="A114" t="s">
         <v>604</v>
       </c>
@@ -15503,10 +15842,10 @@
         <v>1941</v>
       </c>
       <c r="F114" t="s">
-        <v>1869</v>
-      </c>
-    </row>
-    <row r="115" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
       <c r="A115" t="s">
         <v>606</v>
       </c>
@@ -15519,11 +15858,8 @@
       <c r="F115" t="s">
         <v>1869</v>
       </c>
-      <c r="G115" t="s">
-        <v>1874</v>
-      </c>
-    </row>
-    <row r="116" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="116" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
       <c r="A116" t="s">
         <v>608</v>
       </c>
@@ -15533,8 +15869,11 @@
       <c r="E116" t="s">
         <v>1941</v>
       </c>
-    </row>
-    <row r="117" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F116" t="s">
+        <v>1869</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
       <c r="A117" t="s">
         <v>622</v>
       </c>
@@ -15544,8 +15883,11 @@
       <c r="E117" t="s">
         <v>1941</v>
       </c>
-    </row>
-    <row r="118" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F117" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
       <c r="A118" t="s">
         <v>628</v>
       </c>
@@ -15555,8 +15897,11 @@
       <c r="E118" t="s">
         <v>1934</v>
       </c>
-    </row>
-    <row r="119" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F118" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
       <c r="A119" t="s">
         <v>634</v>
       </c>
@@ -15566,8 +15911,11 @@
       <c r="E119" t="s">
         <v>1934</v>
       </c>
-    </row>
-    <row r="120" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F119" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
       <c r="A120" t="s">
         <v>911</v>
       </c>
@@ -15577,8 +15925,11 @@
       <c r="E120" t="s">
         <v>1940</v>
       </c>
-    </row>
-    <row r="121" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F120" t="s">
+        <v>1869</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
       <c r="A121" t="s">
         <v>913</v>
       </c>
@@ -15588,8 +15939,11 @@
       <c r="E121" t="s">
         <v>1940</v>
       </c>
-    </row>
-    <row r="122" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F121" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
       <c r="A122" t="s">
         <v>915</v>
       </c>
@@ -15599,8 +15953,11 @@
       <c r="E122" t="s">
         <v>1940</v>
       </c>
-    </row>
-    <row r="123" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F122" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
       <c r="A123" t="s">
         <v>1068</v>
       </c>
@@ -15610,8 +15967,11 @@
       <c r="E123" t="s">
         <v>1934</v>
       </c>
-    </row>
-    <row r="124" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F123" t="s">
+        <v>1869</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
       <c r="A124" t="s">
         <v>1070</v>
       </c>
@@ -15625,8 +15985,8 @@
         <v>1869</v>
       </c>
     </row>
-    <row r="125" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A125" t="s">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A125" s="9" t="s">
         <v>1166</v>
       </c>
       <c r="B125" t="s">
@@ -15636,14 +15996,11 @@
         <v>171</v>
       </c>
       <c r="F125" t="s">
-        <v>1869</v>
-      </c>
-      <c r="G125" t="s">
-        <v>1873</v>
-      </c>
-    </row>
-    <row r="126" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A126" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A126" s="9" t="s">
         <v>1168</v>
       </c>
       <c r="B126" t="s">
@@ -15653,13 +16010,10 @@
         <v>171</v>
       </c>
       <c r="F126" t="s">
-        <v>1869</v>
-      </c>
-      <c r="G126" t="s">
-        <v>1873</v>
-      </c>
-    </row>
-    <row r="127" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
       <c r="A127" t="s">
         <v>1170</v>
       </c>
@@ -15673,8 +16027,8 @@
         <v>1869</v>
       </c>
     </row>
-    <row r="128" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A128" t="s">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A128" s="9" t="s">
         <v>1284</v>
       </c>
       <c r="B128" t="s">
@@ -15683,8 +16037,11 @@
       <c r="E128" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="129" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F128" t="s">
+        <v>1871</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A129" t="s">
         <v>1505</v>
       </c>
@@ -15694,8 +16051,11 @@
       <c r="E129" t="s">
         <v>1933</v>
       </c>
-    </row>
-    <row r="130" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F129" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A130" t="s">
         <v>1507</v>
       </c>
@@ -15705,8 +16065,11 @@
       <c r="E130" t="s">
         <v>1933</v>
       </c>
-    </row>
-    <row r="131" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F130" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A131" t="s">
         <v>1511</v>
       </c>
@@ -15716,8 +16079,11 @@
       <c r="E131" t="s">
         <v>1933</v>
       </c>
-    </row>
-    <row r="132" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F131" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A132" t="s">
         <v>1513</v>
       </c>
@@ -15727,9 +16093,12 @@
       <c r="E132" t="s">
         <v>1933</v>
       </c>
-    </row>
-    <row r="133" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A133" t="s">
+      <c r="F132" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A133" s="9" t="s">
         <v>1702</v>
       </c>
       <c r="B133" t="s">
@@ -15738,8 +16107,14 @@
       <c r="E133" t="s">
         <v>1937</v>
       </c>
-    </row>
-    <row r="134" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F133" t="s">
+        <v>1870</v>
+      </c>
+      <c r="G133" t="s">
+        <v>1874</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A134" t="s">
         <v>1716</v>
       </c>
@@ -15749,8 +16124,11 @@
       <c r="E134" t="s">
         <v>1948</v>
       </c>
-    </row>
-    <row r="135" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F134" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A135" t="s">
         <v>1718</v>
       </c>
@@ -15760,8 +16138,11 @@
       <c r="E135" t="s">
         <v>1948</v>
       </c>
-    </row>
-    <row r="136" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F135" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A136" t="s">
         <v>1720</v>
       </c>
@@ -15771,8 +16152,11 @@
       <c r="E136" t="s">
         <v>1948</v>
       </c>
-    </row>
-    <row r="137" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F136" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A137" t="s">
         <v>1722</v>
       </c>
@@ -15782,8 +16166,11 @@
       <c r="E137" t="s">
         <v>1948</v>
       </c>
-    </row>
-    <row r="138" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F137" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A138" t="s">
         <v>1724</v>
       </c>
@@ -15793,8 +16180,11 @@
       <c r="E138" t="s">
         <v>1948</v>
       </c>
-    </row>
-    <row r="139" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F138" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A139" t="s">
         <v>1726</v>
       </c>
@@ -15804,8 +16194,11 @@
       <c r="E139" t="s">
         <v>1948</v>
       </c>
-    </row>
-    <row r="140" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F139" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A140" t="s">
         <v>1728</v>
       </c>
@@ -15815,8 +16208,11 @@
       <c r="E140" t="s">
         <v>1948</v>
       </c>
-    </row>
-    <row r="141" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F140" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A141" t="s">
         <v>8</v>
       </c>
@@ -15826,8 +16222,11 @@
       <c r="E141" t="s">
         <v>1938</v>
       </c>
-    </row>
-    <row r="142" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F141" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A142" t="s">
         <v>92</v>
       </c>
@@ -15837,8 +16236,11 @@
       <c r="E142" t="s">
         <v>1943</v>
       </c>
-    </row>
-    <row r="143" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F142" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A143" t="s">
         <v>378</v>
       </c>
@@ -15848,8 +16250,11 @@
       <c r="E143" t="s">
         <v>1934</v>
       </c>
-    </row>
-    <row r="144" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F143" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A144" t="s">
         <v>380</v>
       </c>
@@ -15859,8 +16264,11 @@
       <c r="E144" t="s">
         <v>1934</v>
       </c>
-    </row>
-    <row r="145" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F144" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
       <c r="A145" t="s">
         <v>382</v>
       </c>
@@ -15870,8 +16278,11 @@
       <c r="E145" t="s">
         <v>1934</v>
       </c>
-    </row>
-    <row r="146" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F145" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
       <c r="A146" t="s">
         <v>384</v>
       </c>
@@ -15881,8 +16292,11 @@
       <c r="E146" t="s">
         <v>1934</v>
       </c>
-    </row>
-    <row r="147" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F146" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
       <c r="A147" t="s">
         <v>386</v>
       </c>
@@ -15892,8 +16306,11 @@
       <c r="E147" t="s">
         <v>1934</v>
       </c>
-    </row>
-    <row r="148" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F147" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
       <c r="A148" t="s">
         <v>446</v>
       </c>
@@ -15903,8 +16320,11 @@
       <c r="E148" t="s">
         <v>1934</v>
       </c>
-    </row>
-    <row r="149" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F148" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
       <c r="A149" t="s">
         <v>514</v>
       </c>
@@ -15914,8 +16334,11 @@
       <c r="E149" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="150" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F149" t="s">
+        <v>1869</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
       <c r="A150" t="s">
         <v>526</v>
       </c>
@@ -15925,8 +16348,11 @@
       <c r="E150" t="s">
         <v>1935</v>
       </c>
-    </row>
-    <row r="151" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F150" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
       <c r="A151" t="s">
         <v>528</v>
       </c>
@@ -15936,8 +16362,11 @@
       <c r="E151" t="s">
         <v>1935</v>
       </c>
-    </row>
-    <row r="152" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F151" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
       <c r="A152" t="s">
         <v>530</v>
       </c>
@@ -15947,8 +16376,11 @@
       <c r="E152" t="s">
         <v>1935</v>
       </c>
-    </row>
-    <row r="153" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F152" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
       <c r="A153" t="s">
         <v>532</v>
       </c>
@@ -15958,8 +16390,11 @@
       <c r="E153" t="s">
         <v>1935</v>
       </c>
-    </row>
-    <row r="154" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F153" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
       <c r="A154" t="s">
         <v>534</v>
       </c>
@@ -15969,8 +16404,11 @@
       <c r="E154" t="s">
         <v>1935</v>
       </c>
-    </row>
-    <row r="155" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F154" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
       <c r="A155" t="s">
         <v>536</v>
       </c>
@@ -15980,8 +16418,11 @@
       <c r="E155" t="s">
         <v>1935</v>
       </c>
-    </row>
-    <row r="156" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F155" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
       <c r="A156" t="s">
         <v>538</v>
       </c>
@@ -15991,8 +16432,11 @@
       <c r="E156" t="s">
         <v>1935</v>
       </c>
-    </row>
-    <row r="157" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F156" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
       <c r="A157" t="s">
         <v>540</v>
       </c>
@@ -16002,8 +16446,11 @@
       <c r="E157" t="s">
         <v>1935</v>
       </c>
-    </row>
-    <row r="158" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F157" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
       <c r="A158" t="s">
         <v>542</v>
       </c>
@@ -16013,8 +16460,11 @@
       <c r="E158" t="s">
         <v>1935</v>
       </c>
-    </row>
-    <row r="159" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F158" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
       <c r="A159" t="s">
         <v>544</v>
       </c>
@@ -16024,8 +16474,11 @@
       <c r="E159" t="s">
         <v>1935</v>
       </c>
-    </row>
-    <row r="160" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F159" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
       <c r="A160" t="s">
         <v>546</v>
       </c>
@@ -16035,8 +16488,11 @@
       <c r="E160" t="s">
         <v>1935</v>
       </c>
-    </row>
-    <row r="161" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F160" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
       <c r="A161" t="s">
         <v>548</v>
       </c>
@@ -16046,8 +16502,11 @@
       <c r="E161" t="s">
         <v>1935</v>
       </c>
-    </row>
-    <row r="162" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F161" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
       <c r="A162" t="s">
         <v>550</v>
       </c>
@@ -16057,8 +16516,11 @@
       <c r="E162" t="s">
         <v>1935</v>
       </c>
-    </row>
-    <row r="163" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F162" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
       <c r="A163" t="s">
         <v>552</v>
       </c>
@@ -16068,8 +16530,11 @@
       <c r="E163" t="s">
         <v>1935</v>
       </c>
-    </row>
-    <row r="164" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F163" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
       <c r="A164" t="s">
         <v>554</v>
       </c>
@@ -16079,8 +16544,11 @@
       <c r="E164" t="s">
         <v>1935</v>
       </c>
-    </row>
-    <row r="165" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F164" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
       <c r="A165" t="s">
         <v>556</v>
       </c>
@@ -16090,8 +16558,11 @@
       <c r="E165" t="s">
         <v>1935</v>
       </c>
-    </row>
-    <row r="166" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F165" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
       <c r="A166" t="s">
         <v>558</v>
       </c>
@@ -16101,8 +16572,11 @@
       <c r="E166" t="s">
         <v>1935</v>
       </c>
-    </row>
-    <row r="167" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F166" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
       <c r="A167" t="s">
         <v>560</v>
       </c>
@@ -16112,8 +16586,11 @@
       <c r="E167" t="s">
         <v>1935</v>
       </c>
-    </row>
-    <row r="168" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F167" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
       <c r="A168" t="s">
         <v>648</v>
       </c>
@@ -16123,8 +16600,11 @@
       <c r="E168" t="s">
         <v>1945</v>
       </c>
-    </row>
-    <row r="169" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F168" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
       <c r="A169" t="s">
         <v>650</v>
       </c>
@@ -16134,8 +16614,11 @@
       <c r="E169" t="s">
         <v>1945</v>
       </c>
-    </row>
-    <row r="170" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F169" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
       <c r="A170" t="s">
         <v>652</v>
       </c>
@@ -16145,8 +16628,11 @@
       <c r="E170" t="s">
         <v>1945</v>
       </c>
-    </row>
-    <row r="171" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F170" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
       <c r="A171" t="s">
         <v>654</v>
       </c>
@@ -16156,8 +16642,11 @@
       <c r="E171" t="s">
         <v>1945</v>
       </c>
-    </row>
-    <row r="172" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F171" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
       <c r="A172" t="s">
         <v>656</v>
       </c>
@@ -16167,8 +16656,11 @@
       <c r="E172" t="s">
         <v>1945</v>
       </c>
-    </row>
-    <row r="173" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F172" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
       <c r="A173" t="s">
         <v>658</v>
       </c>
@@ -16178,8 +16670,11 @@
       <c r="E173" t="s">
         <v>1945</v>
       </c>
-    </row>
-    <row r="174" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F173" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
       <c r="A174" t="s">
         <v>662</v>
       </c>
@@ -16189,8 +16684,11 @@
       <c r="E174" t="s">
         <v>1945</v>
       </c>
-    </row>
-    <row r="175" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F174" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
       <c r="A175" t="s">
         <v>664</v>
       </c>
@@ -16200,8 +16698,11 @@
       <c r="E175" t="s">
         <v>1945</v>
       </c>
-    </row>
-    <row r="176" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F175" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
       <c r="A176" t="s">
         <v>666</v>
       </c>
@@ -16211,8 +16712,11 @@
       <c r="E176" t="s">
         <v>1948</v>
       </c>
-    </row>
-    <row r="177" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F176" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="177" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A177" t="s">
         <v>668</v>
       </c>
@@ -16222,8 +16726,11 @@
       <c r="E177" t="s">
         <v>1948</v>
       </c>
-    </row>
-    <row r="178" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F177" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="178" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A178" t="s">
         <v>670</v>
       </c>
@@ -16233,8 +16740,11 @@
       <c r="E178" t="s">
         <v>1948</v>
       </c>
-    </row>
-    <row r="179" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F178" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="179" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A179" t="s">
         <v>697</v>
       </c>
@@ -16244,8 +16754,11 @@
       <c r="E179" t="s">
         <v>1938</v>
       </c>
-    </row>
-    <row r="180" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F179" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="180" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A180" t="s">
         <v>699</v>
       </c>
@@ -16255,8 +16768,11 @@
       <c r="E180" t="s">
         <v>1938</v>
       </c>
-    </row>
-    <row r="181" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F180" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="181" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A181" t="s">
         <v>731</v>
       </c>
@@ -16266,8 +16782,11 @@
       <c r="E181" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="182" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F181" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="182" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A182" t="s">
         <v>733</v>
       </c>
@@ -16277,8 +16796,11 @@
       <c r="E182" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="183" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F182" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="183" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A183" t="s">
         <v>757</v>
       </c>
@@ -16288,8 +16810,11 @@
       <c r="E183" t="s">
         <v>1945</v>
       </c>
-    </row>
-    <row r="184" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F183" t="s">
+        <v>1869</v>
+      </c>
+    </row>
+    <row r="184" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A184" t="s">
         <v>763</v>
       </c>
@@ -16299,8 +16824,11 @@
       <c r="E184" t="s">
         <v>1938</v>
       </c>
-    </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F184" t="s">
+        <v>1869</v>
+      </c>
+    </row>
+    <row r="185" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A185" t="s">
         <v>771</v>
       </c>
@@ -16310,9 +16838,12 @@
       <c r="E185" t="s">
         <v>1936</v>
       </c>
-    </row>
-    <row r="186" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A186" t="s">
+      <c r="F185" t="s">
+        <v>1869</v>
+      </c>
+    </row>
+    <row r="186" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A186" s="9" t="s">
         <v>811</v>
       </c>
       <c r="B186" t="s">
@@ -16321,8 +16852,14 @@
       <c r="E186" t="s">
         <v>1940</v>
       </c>
-    </row>
-    <row r="187" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F186" t="s">
+        <v>1974</v>
+      </c>
+      <c r="G186" t="s">
+        <v>1874</v>
+      </c>
+    </row>
+    <row r="187" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A187" t="s">
         <v>813</v>
       </c>
@@ -16332,8 +16869,11 @@
       <c r="E187" t="s">
         <v>1940</v>
       </c>
-    </row>
-    <row r="188" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F187" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="188" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A188" t="s">
         <v>865</v>
       </c>
@@ -16343,8 +16883,11 @@
       <c r="E188" t="s">
         <v>1940</v>
       </c>
-    </row>
-    <row r="189" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F188" t="s">
+        <v>1869</v>
+      </c>
+    </row>
+    <row r="189" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A189" t="s">
         <v>1062</v>
       </c>
@@ -16354,8 +16897,11 @@
       <c r="E189" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="190" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F189" t="s">
+        <v>1869</v>
+      </c>
+    </row>
+    <row r="190" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A190" t="s">
         <v>1064</v>
       </c>
@@ -16365,8 +16911,11 @@
       <c r="E190" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="191" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F190" t="s">
+        <v>1869</v>
+      </c>
+    </row>
+    <row r="191" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A191" t="s">
         <v>1066</v>
       </c>
@@ -16376,8 +16925,11 @@
       <c r="E191" t="s">
         <v>1934</v>
       </c>
-    </row>
-    <row r="192" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F191" t="s">
+        <v>1869</v>
+      </c>
+    </row>
+    <row r="192" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A192" t="s">
         <v>1072</v>
       </c>
@@ -16387,9 +16939,12 @@
       <c r="E192" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="193" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
-      <c r="A193" t="s">
+      <c r="F192" t="s">
+        <v>1869</v>
+      </c>
+    </row>
+    <row r="193" spans="1:7" ht="71.25" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A193" s="9" t="s">
         <v>1232</v>
       </c>
       <c r="B193" t="s">
@@ -16401,9 +16956,15 @@
       <c r="E193" t="s">
         <v>1936</v>
       </c>
-    </row>
-    <row r="194" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
-      <c r="A194" t="s">
+      <c r="F193" t="s">
+        <v>1870</v>
+      </c>
+      <c r="G193" t="s">
+        <v>1874</v>
+      </c>
+    </row>
+    <row r="194" spans="1:7" ht="71.25" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A194" s="9" t="s">
         <v>1234</v>
       </c>
       <c r="B194" t="s">
@@ -16414,6 +16975,12 @@
       </c>
       <c r="E194" t="s">
         <v>1936</v>
+      </c>
+      <c r="F194" t="s">
+        <v>1870</v>
+      </c>
+      <c r="G194" t="s">
+        <v>1874</v>
       </c>
     </row>
     <row r="195" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
@@ -16426,6 +16993,9 @@
       <c r="E195" t="s">
         <v>1941</v>
       </c>
+      <c r="F195" t="s">
+        <v>1868</v>
+      </c>
     </row>
     <row r="196" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A196" t="s">
@@ -16437,8 +17007,11 @@
       <c r="E196" t="s">
         <v>1941</v>
       </c>
-    </row>
-    <row r="197" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="F196" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="197" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A197" t="s">
         <v>1258</v>
       </c>
@@ -16448,8 +17021,11 @@
       <c r="E197" t="s">
         <v>1936</v>
       </c>
-    </row>
-    <row r="198" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="F197" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="198" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A198" t="s">
         <v>1260</v>
       </c>
@@ -16458,6 +17034,9 @@
       </c>
       <c r="E198" t="s">
         <v>1936</v>
+      </c>
+      <c r="F198" t="s">
+        <v>1868</v>
       </c>
     </row>
     <row r="199" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
@@ -16470,6 +17049,9 @@
       <c r="E199" t="s">
         <v>1938</v>
       </c>
+      <c r="F199" t="s">
+        <v>1868</v>
+      </c>
     </row>
     <row r="200" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A200" t="s">
@@ -16481,6 +17063,9 @@
       <c r="E200" t="s">
         <v>1933</v>
       </c>
+      <c r="F200" t="s">
+        <v>1868</v>
+      </c>
     </row>
     <row r="201" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A201" t="s">
@@ -16492,6 +17077,9 @@
       <c r="E201" t="s">
         <v>1934</v>
       </c>
+      <c r="F201" t="s">
+        <v>1868</v>
+      </c>
     </row>
     <row r="202" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A202" t="s">
@@ -16503,6 +17091,9 @@
       <c r="E202" t="s">
         <v>1934</v>
       </c>
+      <c r="F202" t="s">
+        <v>1868</v>
+      </c>
     </row>
     <row r="203" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A203" t="s">
@@ -16514,9 +17105,12 @@
       <c r="E203" t="s">
         <v>1934</v>
       </c>
+      <c r="F203" t="s">
+        <v>1868</v>
+      </c>
     </row>
     <row r="204" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A204" s="7" t="s">
+      <c r="A204" s="9" t="s">
         <v>1525</v>
       </c>
       <c r="B204" t="s">
@@ -16533,7 +17127,7 @@
       </c>
     </row>
     <row r="205" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A205" t="s">
+      <c r="A205" s="9" t="s">
         <v>1527</v>
       </c>
       <c r="B205" t="s">
@@ -16541,6 +17135,12 @@
       </c>
       <c r="E205" t="s">
         <v>1934</v>
+      </c>
+      <c r="F205" t="s">
+        <v>1870</v>
+      </c>
+      <c r="G205" t="s">
+        <v>1874</v>
       </c>
     </row>
     <row r="206" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
@@ -16553,6 +17153,9 @@
       <c r="E206" t="s">
         <v>1934</v>
       </c>
+      <c r="F206" t="s">
+        <v>1868</v>
+      </c>
     </row>
     <row r="207" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A207" t="s">
@@ -16564,9 +17167,12 @@
       <c r="E207" t="s">
         <v>1934</v>
       </c>
+      <c r="F207" t="s">
+        <v>1868</v>
+      </c>
     </row>
     <row r="208" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A208" t="s">
+      <c r="A208" s="9" t="s">
         <v>1533</v>
       </c>
       <c r="B208" t="s">
@@ -16575,8 +17181,14 @@
       <c r="E208" t="s">
         <v>1945</v>
       </c>
-    </row>
-    <row r="209" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F208" t="s">
+        <v>1870</v>
+      </c>
+      <c r="G208" t="s">
+        <v>1874</v>
+      </c>
+    </row>
+    <row r="209" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A209" t="s">
         <v>1645</v>
       </c>
@@ -16586,9 +17198,12 @@
       <c r="E209" t="s">
         <v>1945</v>
       </c>
-    </row>
-    <row r="210" spans="1:5" ht="71.25" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A210" t="s">
+      <c r="F209" t="s">
+        <v>1869</v>
+      </c>
+    </row>
+    <row r="210" spans="1:7" ht="71.25" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A210" s="9" t="s">
         <v>1647</v>
       </c>
       <c r="B210" t="s">
@@ -16603,8 +17218,14 @@
       <c r="E210" t="s">
         <v>1945</v>
       </c>
-    </row>
-    <row r="211" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F210" t="s">
+        <v>1870</v>
+      </c>
+      <c r="G210" t="s">
+        <v>1874</v>
+      </c>
+    </row>
+    <row r="211" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A211" t="s">
         <v>1657</v>
       </c>
@@ -16614,8 +17235,11 @@
       <c r="E211" t="s">
         <v>1945</v>
       </c>
-    </row>
-    <row r="212" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F211" t="s">
+        <v>1869</v>
+      </c>
+    </row>
+    <row r="212" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A212" t="s">
         <v>1659</v>
       </c>
@@ -16625,8 +17249,11 @@
       <c r="E212" t="s">
         <v>1945</v>
       </c>
-    </row>
-    <row r="213" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F212" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="213" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A213" t="s">
         <v>1661</v>
       </c>
@@ -16636,8 +17263,11 @@
       <c r="E213" t="s">
         <v>1945</v>
       </c>
-    </row>
-    <row r="214" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F213" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="214" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A214" t="s">
         <v>1663</v>
       </c>
@@ -16647,9 +17277,12 @@
       <c r="E214" t="s">
         <v>1945</v>
       </c>
-    </row>
-    <row r="215" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A215" t="s">
+      <c r="F214" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="215" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A215" s="9" t="s">
         <v>1696</v>
       </c>
       <c r="B215" t="s">
@@ -16658,9 +17291,15 @@
       <c r="E215" t="s">
         <v>1946</v>
       </c>
-    </row>
-    <row r="216" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A216" t="s">
+      <c r="F215" t="s">
+        <v>1870</v>
+      </c>
+      <c r="G215" t="s">
+        <v>1874</v>
+      </c>
+    </row>
+    <row r="216" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A216" s="9" t="s">
         <v>1698</v>
       </c>
       <c r="B216" t="s">
@@ -16669,9 +17308,15 @@
       <c r="E216" t="s">
         <v>1946</v>
       </c>
-    </row>
-    <row r="217" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A217" s="7" t="s">
+      <c r="F216" t="s">
+        <v>1870</v>
+      </c>
+      <c r="G216" t="s">
+        <v>1874</v>
+      </c>
+    </row>
+    <row r="217" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A217" s="9" t="s">
         <v>1700</v>
       </c>
       <c r="B217" t="s">
@@ -16680,9 +17325,12 @@
       <c r="E217" t="s">
         <v>1946</v>
       </c>
-    </row>
-    <row r="218" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A218" s="7" t="s">
+      <c r="F217" t="s">
+        <v>1869</v>
+      </c>
+    </row>
+    <row r="218" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A218" s="9" t="s">
         <v>1704</v>
       </c>
       <c r="B218" t="s">
@@ -16691,8 +17339,11 @@
       <c r="E218" t="s">
         <v>1946</v>
       </c>
-    </row>
-    <row r="219" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F218" t="s">
+        <v>1869</v>
+      </c>
+    </row>
+    <row r="219" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A219" t="s">
         <v>1714</v>
       </c>
@@ -16702,9 +17353,12 @@
       <c r="E219" t="s">
         <v>1945</v>
       </c>
-    </row>
-    <row r="220" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A220" s="7" t="s">
+      <c r="F219" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="220" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A220" s="9" t="s">
         <v>1780</v>
       </c>
       <c r="B220" t="s">
@@ -16713,9 +17367,15 @@
       <c r="E220" t="s">
         <v>1937</v>
       </c>
-    </row>
-    <row r="221" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A221" s="7" t="s">
+      <c r="F220" t="s">
+        <v>1870</v>
+      </c>
+      <c r="G220" t="s">
+        <v>1874</v>
+      </c>
+    </row>
+    <row r="221" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A221" s="9" t="s">
         <v>1782</v>
       </c>
       <c r="B221" t="s">
@@ -16724,8 +17384,14 @@
       <c r="E221" t="s">
         <v>1937</v>
       </c>
-    </row>
-    <row r="222" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F221" t="s">
+        <v>1870</v>
+      </c>
+      <c r="G221" t="s">
+        <v>1874</v>
+      </c>
+    </row>
+    <row r="222" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A222" t="s">
         <v>1784</v>
       </c>
@@ -16735,8 +17401,11 @@
       <c r="E222" t="s">
         <v>1933</v>
       </c>
-    </row>
-    <row r="223" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F222" t="s">
+        <v>1869</v>
+      </c>
+    </row>
+    <row r="223" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A223" t="s">
         <v>1786</v>
       </c>
@@ -16746,8 +17415,11 @@
       <c r="E223" t="s">
         <v>1937</v>
       </c>
-    </row>
-    <row r="224" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F223" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="224" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A224" t="s">
         <v>1788</v>
       </c>
@@ -16757,8 +17429,11 @@
       <c r="E224" t="s">
         <v>1937</v>
       </c>
-    </row>
-    <row r="225" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F224" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="225" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
       <c r="A225" t="s">
         <v>1790</v>
       </c>
@@ -16768,8 +17443,11 @@
       <c r="E225" t="s">
         <v>1937</v>
       </c>
-    </row>
-    <row r="226" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F225" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="226" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
       <c r="A226" t="s">
         <v>1792</v>
       </c>
@@ -16779,8 +17457,11 @@
       <c r="E226" t="s">
         <v>1937</v>
       </c>
-    </row>
-    <row r="227" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F226" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="227" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
       <c r="A227" t="s">
         <v>1794</v>
       </c>
@@ -16790,8 +17471,11 @@
       <c r="E227" t="s">
         <v>1937</v>
       </c>
-    </row>
-    <row r="228" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F227" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="228" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
       <c r="A228" t="s">
         <v>1796</v>
       </c>
@@ -16801,8 +17485,11 @@
       <c r="E228" t="s">
         <v>1937</v>
       </c>
-    </row>
-    <row r="229" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F228" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="229" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
       <c r="A229" t="s">
         <v>1798</v>
       </c>
@@ -16812,8 +17499,11 @@
       <c r="E229" t="s">
         <v>1937</v>
       </c>
-    </row>
-    <row r="230" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F229" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="230" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
       <c r="A230" t="s">
         <v>1800</v>
       </c>
@@ -16823,8 +17513,11 @@
       <c r="E230" t="s">
         <v>1937</v>
       </c>
-    </row>
-    <row r="231" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+      <c r="F230" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="231" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
       <c r="A231" t="s">
         <v>1802</v>
       </c>
@@ -16834,13 +17527,21 @@
       <c r="E231" t="s">
         <v>1937</v>
       </c>
+      <c r="F231" t="s">
+        <v>1868</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H231" xr:uid="{DDF76284-18C6-40F6-BB15-A93600E21133}">
-    <filterColumn colId="4">
+  <autoFilter ref="A1:I231" xr:uid="{DDF76284-18C6-40F6-BB15-A93600E21133}">
+    <filterColumn colId="5">
       <filters>
-        <filter val="Socail - Friends"/>
+        <filter val="For Calculation"/>
+        <filter val="For model"/>
+        <filter val="For plot"/>
       </filters>
+    </filterColumn>
+    <filterColumn colId="6">
+      <filters blank="1"/>
     </filterColumn>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -16856,7 +17557,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{215134CD-200E-4679-BC43-8B986D56DED7}">
           <x14:formula1>
-            <xm:f>Types!$B$2:$B$5</xm:f>
+            <xm:f>Types!$B$2:$B$7</xm:f>
           </x14:formula1>
           <xm:sqref>F1:F1048576</xm:sqref>
         </x14:dataValidation>
@@ -16883,7 +17584,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16:B17"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -16992,6 +17693,9 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B6" t="s">
+        <v>1974</v>
+      </c>
       <c r="D6" t="s">
         <v>1953</v>
       </c>
@@ -17312,18 +18016,18 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7B17E8F-9228-4F03-B401-83ABEE385989}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="22.265625" customWidth="1"/>
+    <col min="1" max="1" width="43.3984375" customWidth="1"/>
     <col min="2" max="2" width="53.73046875" customWidth="1"/>
     <col min="3" max="3" width="27.265625" customWidth="1"/>
-    <col min="4" max="4" width="29.1328125" customWidth="1"/>
+    <col min="4" max="4" width="37.1328125" customWidth="1"/>
     <col min="5" max="5" width="13" customWidth="1"/>
     <col min="6" max="6" width="79.86328125" customWidth="1"/>
   </cols>
@@ -17371,7 +18075,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="156.75" x14ac:dyDescent="0.45">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
         <v>1965</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -17380,7 +18084,7 @@
       <c r="C4" s="5" t="s">
         <v>1880</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="7" t="s">
         <v>1968</v>
       </c>
       <c r="E4" s="5"/>
@@ -17394,6 +18098,50 @@
       </c>
       <c r="D5" s="4" t="s">
         <v>1971</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="99.75" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>1976</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1881</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>1980</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="128.25" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>1977</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1881</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>1981</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="128.25" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>1978</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1881</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>1982</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="213.75" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>1979</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1881</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>1983</v>
       </c>
     </row>
   </sheetData>

</xml_diff>